<commit_message>
atualização de tempos e algoritmo dígito de controlo
</commit_message>
<xml_diff>
--- a/IPGtrails4health/doc/Tempos.xlsx
+++ b/IPGtrails4health/doc/Tempos.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1012177\Desktop\IPGtrails4health\IPGtrails4health\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\IPGtrails4health\IPGtrails4health\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -312,39 +312,45 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -352,12 +358,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,11 +674,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:S46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8:O9"/>
+      <selection activeCell="Q6" sqref="Q6:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,46 +689,46 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="14"/>
+      <c r="L2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="14"/>
+      <c r="N2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="5" t="s">
+      <c r="O2" s="14"/>
+      <c r="P2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="5" t="s">
+      <c r="Q2" s="14"/>
+      <c r="R2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="6"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="2:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
@@ -779,202 +779,210 @@
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="14">
+      <c r="C4" s="12"/>
+      <c r="D4" s="5">
         <v>0.5</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="5">
         <v>0.5</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="5">
         <v>0</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="5">
         <v>0</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="5">
         <v>1</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="5">
         <v>0</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="5">
         <v>0.5</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="5">
         <v>0</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="5">
         <v>1.5</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="5">
         <v>0.5</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="5">
         <v>1.5</v>
       </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="15"/>
+      <c r="P4" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="15"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="16">
+      <c r="C6" s="12"/>
+      <c r="D6" s="18">
         <v>0.5</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="5">
         <v>0.5</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="5">
         <v>0</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="5">
         <v>0</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="5">
         <v>1</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="5">
         <v>0</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="5">
         <v>0</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="5">
         <v>1.5</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="5">
         <v>0.5</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="5">
         <v>1.5</v>
       </c>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="15"/>
+      <c r="P6" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>1</v>
+      </c>
+      <c r="R6" s="5"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="16">
+      <c r="C8" s="12"/>
+      <c r="D8" s="18">
         <v>0.5</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="5">
         <v>0.5</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="5">
         <v>0</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="5">
         <v>1</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="5">
         <v>0</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="5">
         <v>1</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="5">
         <v>0</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="5">
         <v>0.5</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="5">
         <v>0</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="5">
         <v>1.5</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="5">
         <v>0.5</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="5">
         <v>1.5</v>
       </c>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
+      <c r="P8" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="20"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="8"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
@@ -1681,6 +1689,50 @@
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="B2:C3"/>
@@ -1697,50 +1749,6 @@
     <mergeCell ref="J8:J9"/>
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>